<commit_message>
acabando o robo de pedido de emprestimo
</commit_message>
<xml_diff>
--- a/Processamento de Pedidos de Empréstimo/PedidosEmprestimo.xlsx
+++ b/Processamento de Pedidos de Empréstimo/PedidosEmprestimo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marce\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CATALOG\Documents\UiPath\RPA_UdemyMarceloCruz\Processamento de Pedidos de Empréstimo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BF4E05F-E07D-4476-A7FA-C4D6E5EAFE90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48160F4C-2263-495F-BECD-FCF816A6B12F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="15375" windowHeight="7995" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pedidos" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
   <si>
     <t>APR</t>
   </si>
@@ -67,6 +67,24 @@
   </si>
   <si>
     <t>marcelo@teste.com</t>
+  </si>
+  <si>
+    <t>Aprovado</t>
+  </si>
+  <si>
+    <t>63e52e90eafc1b6d9838f965</t>
+  </si>
+  <si>
+    <t>63e52e98eafc1b6d9838f966</t>
+  </si>
+  <si>
+    <t>63e52ea0eafc1b6d9838f967</t>
+  </si>
+  <si>
+    <t>63e52ea9eafc1b6d9838f968</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Não Aprovado</t>
   </si>
 </sst>
 </file>
@@ -127,7 +145,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -412,17 +430,17 @@
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="37.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -448,7 +466,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -464,8 +482,17 @@
       <c r="E2">
         <v>20</v>
       </c>
+      <c r="F2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2">
+        <v>8</v>
+      </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -481,8 +508,17 @@
       <c r="E3">
         <v>30</v>
       </c>
+      <c r="F3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3">
+        <v>4</v>
+      </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -498,8 +534,17 @@
       <c r="E4">
         <v>45</v>
       </c>
+      <c r="F4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4">
+        <v>9</v>
+      </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
@@ -515,8 +560,17 @@
       <c r="E5">
         <v>29</v>
       </c>
+      <c r="F5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5">
+        <v>8</v>
+      </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
@@ -532,8 +586,11 @@
       <c r="E6">
         <v>70</v>
       </c>
+      <c r="F6" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
@@ -548,6 +605,9 @@
       </c>
       <c r="E7">
         <v>21</v>
+      </c>
+      <c r="F7" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>